<commit_message>
generate report for permanet employee
</commit_message>
<xml_diff>
--- a/pages/payslip/casual/casual_employees_report.xlsx
+++ b/pages/payslip/casual/casual_employees_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
   <si>
     <t>San Mateo, Rizal</t>
   </si>
@@ -50,15 +50,36 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Malejana, Hector Pulido</t>
+  </si>
+  <si>
+    <t>04/24/2024</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>3rd Level</t>
+  </si>
+  <si>
+    <t>Job Order</t>
+  </si>
+  <si>
+    <t>IT Services</t>
+  </si>
+  <si>
+    <t>Lead Technician</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
     <t>Jacinto, Arvin Jeff Ramota</t>
   </si>
   <si>
     <t>12/26/2024</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>No Eligibility</t>
   </si>
   <si>
@@ -71,9 +92,6 @@
     <t>Cleaner</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Cadaoas, Haydee Tomagan</t>
   </si>
   <si>
@@ -83,12 +101,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>3rd Level</t>
-  </si>
-  <si>
-    <t>Job Order</t>
-  </si>
-  <si>
     <t>Others</t>
   </si>
   <si>
@@ -183,9 +195,6 @@
   </si>
   <si>
     <t>09/25/1991</t>
-  </si>
-  <si>
-    <t>IT Services</t>
   </si>
   <si>
     <t>IT Programmer</t>
@@ -601,10 +610,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
@@ -723,22 +732,22 @@
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>18</v>
@@ -746,22 +755,22 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -784,13 +793,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>32</v>
@@ -810,19 +819,19 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>37</v>
@@ -839,13 +848,13 @@
         <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F10" s="2">
         <v>3</v>
@@ -854,7 +863,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>18</v>
@@ -862,28 +871,28 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>18</v>
@@ -891,25 +900,25 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>47</v>
@@ -926,22 +935,22 @@
         <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>18</v>
@@ -949,28 +958,28 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>18</v>
@@ -978,7 +987,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>55</v>
@@ -987,13 +996,13 @@
         <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F15" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>56</v>
@@ -1016,19 +1025,19 @@
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>18</v>
@@ -1036,25 +1045,25 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>64</v>
@@ -1065,28 +1074,28 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>18</v>
@@ -1094,28 +1103,28 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>18</v>
@@ -1123,25 +1132,25 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>70</v>
@@ -1158,35 +1167,64 @@
         <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="2">
+        <v>8</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>3</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
form validation on fields patch
</commit_message>
<xml_diff>
--- a/pages/payslip/casual/casual_employees_report.xlsx
+++ b/pages/payslip/casual/casual_employees_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>San Mateo, Rizal</t>
   </si>
@@ -50,153 +50,141 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Malejana, Hector Pulido</t>
+    <t>De Guzman, Melani San Jose</t>
   </si>
   <si>
     <t>04/24/2024</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>3rd Level</t>
+  </si>
+  <si>
+    <t>Job Order</t>
+  </si>
+  <si>
+    <t>Clerical Services</t>
+  </si>
+  <si>
+    <t>Clerk</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Dorado, Eduardo Fernandez</t>
+  </si>
+  <si>
+    <t>04/26/2024</t>
+  </si>
+  <si>
+    <t>1st Level</t>
+  </si>
+  <si>
+    <t>Casual</t>
+  </si>
+  <si>
+    <t>Health and Allied Services</t>
+  </si>
+  <si>
+    <t>Doctors</t>
+  </si>
+  <si>
+    <t>Jacinto, Arvin Jeff Ramota</t>
+  </si>
+  <si>
+    <t>12/26/2024</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>3rd Level</t>
-  </si>
-  <si>
-    <t>Job Order</t>
+    <t>No Eligibility</t>
+  </si>
+  <si>
+    <t>Janitorial Services</t>
+  </si>
+  <si>
+    <t>Cleaner</t>
+  </si>
+  <si>
+    <t>San Jose, Joan San Jose</t>
+  </si>
+  <si>
+    <t>08/24/1998</t>
+  </si>
+  <si>
+    <t>Doctorr</t>
+  </si>
+  <si>
+    <t>Briones, Eugenio Custodio</t>
+  </si>
+  <si>
+    <t>10/09/2024</t>
+  </si>
+  <si>
+    <t>Technical Services</t>
+  </si>
+  <si>
+    <t>CCTV Installer</t>
+  </si>
+  <si>
+    <t>Sia-Encinares, Aleth Marie Hipolito</t>
+  </si>
+  <si>
+    <t>06/13/2024</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Buay, John Carlo Bonina</t>
+  </si>
+  <si>
+    <t>03/06/2024</t>
+  </si>
+  <si>
+    <t>LED Wall Tech</t>
+  </si>
+  <si>
+    <t>Cruz, Cristina Vergara</t>
+  </si>
+  <si>
+    <t>01/19/1996</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Acang, Mark Anthony Apostol</t>
+  </si>
+  <si>
+    <t>07/29/2024</t>
+  </si>
+  <si>
+    <t>House Plate Installer</t>
+  </si>
+  <si>
+    <t>04/11/2024</t>
+  </si>
+  <si>
+    <t>Security Services</t>
+  </si>
+  <si>
+    <t>Head Security</t>
+  </si>
+  <si>
+    <t>Dolorito, Eddan James Mendoza</t>
+  </si>
+  <si>
+    <t>09/25/1991</t>
   </si>
   <si>
     <t>IT Services</t>
   </si>
   <si>
-    <t>Lead Technician</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Jacinto, Arvin Jeff Ramota</t>
-  </si>
-  <si>
-    <t>12/26/2024</t>
-  </si>
-  <si>
-    <t>No Eligibility</t>
-  </si>
-  <si>
-    <t>Casual</t>
-  </si>
-  <si>
-    <t>Janitorial Services</t>
-  </si>
-  <si>
-    <t>Cleaner</t>
-  </si>
-  <si>
-    <t>Cadaoas, Haydee Tomagan</t>
-  </si>
-  <si>
-    <t>01/16/2024</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>Admin Head</t>
-  </si>
-  <si>
-    <t>San Jose, Joan San Jose</t>
-  </si>
-  <si>
-    <t>08/24/1998</t>
-  </si>
-  <si>
-    <t>Health and Allied Services</t>
-  </si>
-  <si>
-    <t>Doctorr</t>
-  </si>
-  <si>
-    <t>Briones, Eugenio Custodio</t>
-  </si>
-  <si>
-    <t>10/09/2024</t>
-  </si>
-  <si>
-    <t>Technical Services</t>
-  </si>
-  <si>
-    <t>CCTV Installer</t>
-  </si>
-  <si>
-    <t>Sia-Encinares, Aleth Marie Hipolito</t>
-  </si>
-  <si>
-    <t>06/13/2024</t>
-  </si>
-  <si>
-    <t>1st Level</t>
-  </si>
-  <si>
-    <t>Nurse</t>
-  </si>
-  <si>
-    <t>Dorado, Eduardo Fernandez</t>
-  </si>
-  <si>
-    <t>04/19/2024</t>
-  </si>
-  <si>
-    <t>Department Head</t>
-  </si>
-  <si>
-    <t>Buay, John Carlo Bonina</t>
-  </si>
-  <si>
-    <t>03/06/2024</t>
-  </si>
-  <si>
-    <t>LED Wall Tech</t>
-  </si>
-  <si>
-    <t>Cruz, Cristina Vergara</t>
-  </si>
-  <si>
-    <t>01/19/1996</t>
-  </si>
-  <si>
-    <t>Clerical Services</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Acang, Mark Anthony Apostol</t>
-  </si>
-  <si>
-    <t>07/29/2024</t>
-  </si>
-  <si>
-    <t>House Plate Installer</t>
-  </si>
-  <si>
-    <t>04/11/2024</t>
-  </si>
-  <si>
-    <t>Security Services</t>
-  </si>
-  <si>
-    <t>Head Security</t>
-  </si>
-  <si>
-    <t>Dolorito, Eddan James Mendoza</t>
-  </si>
-  <si>
-    <t>09/25/1991</t>
-  </si>
-  <si>
     <t>IT Programmer</t>
   </si>
   <si>
@@ -234,9 +222,6 @@
   </si>
   <si>
     <t>11/12/1980</t>
-  </si>
-  <si>
-    <t>Clerk</t>
   </si>
   <si>
     <t>Rodriguez, Robert Mendoza</t>
@@ -610,10 +595,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -712,7 +697,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
@@ -741,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>23</v>
@@ -764,19 +749,19 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>18</v>
@@ -784,13 +769,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
@@ -802,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>33</v>
@@ -819,7 +804,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
@@ -848,10 +833,10 @@
         <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>22</v>
@@ -860,10 +845,10 @@
         <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>18</v>
@@ -871,28 +856,28 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>18</v>
@@ -900,16 +885,16 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
@@ -918,10 +903,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>18</v>
@@ -929,28 +914,28 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>18</v>
@@ -958,28 +943,28 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="2">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>18</v>
@@ -987,28 +972,28 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>18</v>
@@ -1016,25 +1001,25 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>60</v>
@@ -1054,19 +1039,19 @@
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>18</v>
@@ -1074,28 +1059,28 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>18</v>
@@ -1103,16 +1088,16 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>15</v>
@@ -1124,7 +1109,7 @@
         <v>23</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>18</v>
@@ -1132,28 +1117,28 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F20" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>18</v>
@@ -1161,70 +1146,41 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F21" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>73</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="2">
-        <v>3</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="I22" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>